<commit_message>
changes before stripping drift index
going to remove the drift level SM filtering
</commit_message>
<xml_diff>
--- a/Monk-manuscript/Model_selection.xlsx
+++ b/Monk-manuscript/Model_selection.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melissa.monk\Documents\GitHub\habitat-indices-paper\Monk-manuscript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD50CC4E-4867-4397-BA22-9E10F431958D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF946D8-E11A-4124-AEA6-264A4CCD9CBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" tabRatio="879" xr2:uid="{89F9B152-6796-4838-A514-CE9DBFB6F799}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="4068" tabRatio="879" xr2:uid="{89F9B152-6796-4838-A514-CE9DBFB6F799}"/>
   </bookViews>
   <sheets>
     <sheet name="Black rockfish" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="22">
   <si>
     <t>Model</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>AIC</t>
+  </si>
+  <si>
+    <t>YEAR</t>
   </si>
 </sst>
 </file>
@@ -490,30 +493,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F827E28-5576-4EC4-BF78-90D1429C148D}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9:H11"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G1"/>
       <c r="H1"/>
     </row>
-    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -536,7 +539,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -559,7 +562,7 @@
         <v>8352</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -582,7 +585,7 @@
         <v>8170</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>10</v>
       </c>
@@ -599,7 +602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -616,13 +619,13 @@
         <v>188.93530000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -633,7 +636,7 @@
       <c r="G8"/>
       <c r="H8"/>
     </row>
-    <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
@@ -652,7 +655,7 @@
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -670,7 +673,7 @@
       </c>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -688,7 +691,7 @@
       </c>
       <c r="H11" s="8"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -705,7 +708,7 @@
         <v>47.161900000000102</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -722,7 +725,7 @@
         <v>236.09719999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>13</v>
       </c>
@@ -739,13 +742,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -756,7 +759,7 @@
       <c r="G16"/>
       <c r="H16"/>
     </row>
-    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>0</v>
       </c>
@@ -779,204 +782,238 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>1</v>
       </c>
       <c r="B18" s="8">
-        <v>6675.0973999999997</v>
+        <v>3782.9812999999999</v>
       </c>
       <c r="C18" s="8">
-        <v>7692.0438999999997</v>
+        <v>2526.8458999999998</v>
       </c>
       <c r="D18" s="8">
-        <v>1213.4652000000001</v>
+        <v>751.8306</v>
       </c>
       <c r="E18" s="8">
-        <v>454.39949999999999</v>
+        <v>73.080499999999603</v>
       </c>
       <c r="G18" t="s">
         <v>18</v>
       </c>
       <c r="H18" s="8">
-        <v>9219</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+        <v>2923</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B19" s="8">
-        <v>5497.8936000000003</v>
+        <v>3715.2840000000001</v>
       </c>
       <c r="C19" s="8">
-        <v>7245.2439000000004</v>
+        <v>2476.8384000000001</v>
       </c>
       <c r="D19" s="8">
-        <v>36.2614000000003</v>
+        <v>684.13329999999996</v>
       </c>
       <c r="E19" s="8">
-        <v>7.5995000000002602</v>
+        <v>23.072999999999901</v>
       </c>
       <c r="G19" t="s">
         <v>19</v>
       </c>
-      <c r="H19" s="8">
-        <v>9076</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="12" t="s">
+      <c r="H19" s="9">
+        <v>2881</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="8">
+        <v>3050.1219000000001</v>
+      </c>
+      <c r="C20" s="8">
+        <v>2455.2782000000002</v>
+      </c>
+      <c r="D20" s="8">
+        <v>18.9712</v>
+      </c>
+      <c r="E20" s="8">
+        <v>1.5127999999999699</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="13">
-        <v>5461.6322</v>
-      </c>
-      <c r="C20" s="13">
-        <v>7237.6444000000001</v>
-      </c>
-      <c r="D20" s="13">
-        <v>0</v>
-      </c>
-      <c r="E20" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+      <c r="B21" s="13">
+        <v>3031.1507000000001</v>
+      </c>
+      <c r="C21" s="13">
+        <v>2453.7654000000002</v>
+      </c>
+      <c r="D21" s="13">
+        <v>0</v>
+      </c>
+      <c r="E21" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="8">
-        <v>6404.4958999999999</v>
-      </c>
-      <c r="C21" s="8">
-        <v>7526.1040000000003</v>
-      </c>
-      <c r="D21" s="8">
-        <v>942.86369999999999</v>
-      </c>
-      <c r="E21" s="8">
-        <v>288.45960000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
+      <c r="B22" s="8">
+        <v>3666.0646000000002</v>
+      </c>
+      <c r="C22" s="8">
+        <v>2471.5165999999999</v>
+      </c>
+      <c r="D22" s="8">
+        <v>634.91390000000001</v>
+      </c>
+      <c r="E22" s="8">
+        <v>17.751199999999699</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="G23"/>
-      <c r="H23"/>
-    </row>
-    <row r="24" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="10" t="s">
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="G24"/>
+      <c r="H24"/>
+    </row>
+    <row r="25" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D25" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E25" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G25" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="H25" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="3">
-        <v>1</v>
-      </c>
-      <c r="B25" s="8">
-        <v>1011.274</v>
-      </c>
-      <c r="C25" s="8">
-        <v>2788.6493999999998</v>
-      </c>
-      <c r="D25" s="8">
-        <v>136.2208</v>
-      </c>
-      <c r="E25" s="8">
-        <v>346.75099999999998</v>
-      </c>
-      <c r="G25" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>1</v>
+      </c>
+      <c r="B26" s="8">
+        <v>874.78899999999999</v>
+      </c>
+      <c r="C26" s="8">
+        <v>2128.5128</v>
+      </c>
+      <c r="D26" s="8">
+        <v>207.11250000000001</v>
+      </c>
+      <c r="E26" s="8">
+        <v>185.9145</v>
+      </c>
+      <c r="G26" t="s">
         <v>18</v>
       </c>
-      <c r="H25" s="8">
-        <v>2434</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
+      <c r="H26" s="9">
+        <v>1939</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="8">
+        <v>863.83240000000001</v>
+      </c>
+      <c r="C27" s="8">
+        <v>2085.2001</v>
+      </c>
+      <c r="D27" s="8">
+        <v>196.1559</v>
+      </c>
+      <c r="E27" s="8">
+        <v>142.6018</v>
+      </c>
+      <c r="G27" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" s="8">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="8">
-        <v>889.86249999999995</v>
-      </c>
-      <c r="C26" s="8">
-        <v>2448.6523000000002</v>
-      </c>
-      <c r="D26" s="8">
-        <v>14.8093</v>
-      </c>
-      <c r="E26" s="8">
-        <v>6.7539000000001597</v>
-      </c>
-      <c r="G26" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="8">
-        <v>2507</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="12" t="s">
+      <c r="B28" s="8">
+        <v>676.5204</v>
+      </c>
+      <c r="C28" s="8">
+        <v>1947.0467000000001</v>
+      </c>
+      <c r="D28" s="8">
+        <v>8.8438999999999606</v>
+      </c>
+      <c r="E28" s="8">
+        <v>4.4483999999999897</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="13">
-        <v>875.05319999999995</v>
-      </c>
-      <c r="C27" s="13">
-        <v>2441.8984</v>
-      </c>
-      <c r="D27" s="13">
-        <v>0</v>
-      </c>
-      <c r="E27" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
+      <c r="B29" s="13">
+        <v>667.67650000000003</v>
+      </c>
+      <c r="C29" s="13">
+        <v>1942.5983000000001</v>
+      </c>
+      <c r="D29" s="13">
+        <v>0</v>
+      </c>
+      <c r="E29" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="8">
-        <v>981.48119999999994</v>
-      </c>
-      <c r="C28" s="8">
-        <v>2720.0369999999998</v>
-      </c>
-      <c r="D28" s="8">
-        <v>106.428</v>
-      </c>
-      <c r="E28" s="8">
-        <v>278.1386</v>
+      <c r="B30" s="8">
+        <v>855.0172</v>
+      </c>
+      <c r="C30" s="8">
+        <v>2076.1723999999999</v>
+      </c>
+      <c r="D30" s="8">
+        <v>187.3407</v>
+      </c>
+      <c r="E30" s="8">
+        <v>133.57409999999999</v>
       </c>
     </row>
   </sheetData>
@@ -987,24 +1024,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C170A21-6F84-4949-9751-62A5FA7B2134}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9:I11"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -1013,7 +1050,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1036,7 +1073,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1059,7 +1096,7 @@
         <v>21081</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1082,7 +1119,7 @@
         <v>20546</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>10</v>
       </c>
@@ -1099,7 +1136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1116,13 +1153,13 @@
         <v>146.97450000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1131,7 +1168,7 @@
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
@@ -1150,7 +1187,7 @@
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -1168,7 +1205,7 @@
       </c>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -1186,7 +1223,7 @@
       </c>
       <c r="H11" s="8"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -1203,7 +1240,7 @@
         <v>273.422699999999</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1220,7 +1257,7 @@
         <v>420.39719999999897</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>13</v>
       </c>
@@ -1237,13 +1274,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -1252,7 +1289,7 @@
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>0</v>
       </c>
@@ -1275,202 +1312,236 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>1</v>
       </c>
       <c r="B18" s="8">
-        <v>12440.195400000001</v>
+        <v>10046.955099999999</v>
       </c>
       <c r="C18" s="8">
-        <v>20155.185099999999</v>
+        <v>12222.092199999999</v>
       </c>
       <c r="D18" s="8">
-        <v>1449.6306</v>
+        <v>1129.0382</v>
       </c>
       <c r="E18" s="8">
-        <v>813.86659999999995</v>
+        <v>588.90779999999904</v>
       </c>
       <c r="G18" t="s">
         <v>18</v>
       </c>
       <c r="H18" s="8">
-        <v>23517</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13902</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="8">
-        <v>11076.5656</v>
-      </c>
-      <c r="C19" s="8">
-        <v>19451.881700000002</v>
-      </c>
-      <c r="D19" s="8">
-        <v>86.000799999999998</v>
-      </c>
-      <c r="E19" s="8">
-        <v>110.56319999999999</v>
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>9154.3814999999995</v>
+      </c>
+      <c r="C19">
+        <v>11841.718800000001</v>
+      </c>
+      <c r="D19">
+        <v>236.464599999999</v>
+      </c>
+      <c r="E19">
+        <v>208.53440000000001</v>
       </c>
       <c r="G19" t="s">
         <v>19</v>
       </c>
-      <c r="H19" s="8">
-        <v>22888</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="12" t="s">
+      <c r="H19" s="9">
+        <v>13602</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="8">
+        <v>8964.8507000000009</v>
+      </c>
+      <c r="C20" s="8">
+        <v>11693.820900000001</v>
+      </c>
+      <c r="D20" s="8">
+        <v>46.933800000000701</v>
+      </c>
+      <c r="E20" s="8">
+        <v>60.636500000000503</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="13">
-        <v>10990.5648</v>
-      </c>
-      <c r="C20" s="13">
-        <v>19341.318500000001</v>
-      </c>
-      <c r="D20" s="13">
-        <v>0</v>
-      </c>
-      <c r="E20" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+      <c r="B21" s="13">
+        <v>8917.9169000000002</v>
+      </c>
+      <c r="C21" s="13">
+        <v>11633.1844</v>
+      </c>
+      <c r="D21" s="13">
+        <v>0</v>
+      </c>
+      <c r="E21" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="8">
-        <v>11229.6446</v>
-      </c>
-      <c r="C21" s="8">
-        <v>19502.165499999999</v>
-      </c>
-      <c r="D21" s="8">
-        <v>239.07980000000001</v>
-      </c>
-      <c r="E21" s="8">
-        <v>160.84700000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
+      <c r="B22" s="8">
+        <v>9118.4172999999992</v>
+      </c>
+      <c r="C22" s="8">
+        <v>11775.2709</v>
+      </c>
+      <c r="D22" s="8">
+        <v>200.50039999999899</v>
+      </c>
+      <c r="E22" s="8">
+        <v>142.08649999999901</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="10" t="s">
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D25" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E25" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G25" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="H25" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="3">
-        <v>1</v>
-      </c>
-      <c r="B25" s="8">
-        <v>1110.6768999999999</v>
-      </c>
-      <c r="C25" s="8">
-        <v>7546.4750999999997</v>
-      </c>
-      <c r="D25" s="8">
-        <v>142.33279999999999</v>
-      </c>
-      <c r="E25" s="8">
-        <v>526.04169999999999</v>
-      </c>
-      <c r="G25" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>1</v>
+      </c>
+      <c r="B26" s="8">
+        <v>1084.2655999999999</v>
+      </c>
+      <c r="C26" s="8">
+        <v>7031.9186</v>
+      </c>
+      <c r="D26" s="8">
+        <v>138.28790000000001</v>
+      </c>
+      <c r="E26" s="8">
+        <v>471.57470000000001</v>
+      </c>
+      <c r="G26" t="s">
         <v>18</v>
       </c>
-      <c r="H25" s="8">
-        <v>2435</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
+      <c r="H26" s="9">
+        <v>6549</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27">
+        <v>994.1721</v>
+      </c>
+      <c r="C27">
+        <v>6704.7614999999996</v>
+      </c>
+      <c r="D27">
+        <v>48.194400000000002</v>
+      </c>
+      <c r="E27">
+        <v>144.41759999999999</v>
+      </c>
+      <c r="G27" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" s="8">
+        <v>6713</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="8">
-        <v>983.00810000000001</v>
-      </c>
-      <c r="C26" s="8">
-        <v>7043.0232999999998</v>
-      </c>
-      <c r="D26" s="8">
-        <v>14.664</v>
-      </c>
-      <c r="E26" s="8">
-        <v>22.5899</v>
-      </c>
-      <c r="G26" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="8">
-        <v>2507</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="12" t="s">
+      <c r="B28" s="8">
+        <v>959.92700000000002</v>
+      </c>
+      <c r="C28" s="8">
+        <v>6581.2075999999997</v>
+      </c>
+      <c r="D28" s="8">
+        <v>13.949299999999999</v>
+      </c>
+      <c r="E28" s="8">
+        <v>20.863699999999898</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="13">
-        <v>968.34410000000003</v>
-      </c>
-      <c r="C27" s="13">
-        <v>7020.4333999999999</v>
-      </c>
-      <c r="D27" s="13">
-        <v>0</v>
-      </c>
-      <c r="E27" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
+      <c r="B29" s="13">
+        <v>945.97770000000003</v>
+      </c>
+      <c r="C29" s="13">
+        <v>6560.3438999999998</v>
+      </c>
+      <c r="D29" s="13">
+        <v>0</v>
+      </c>
+      <c r="E29" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="8">
-        <v>1007.4863</v>
-      </c>
-      <c r="C28" s="8">
-        <v>7163.4355999999998</v>
-      </c>
-      <c r="D28" s="8">
-        <v>39.142200000000003</v>
-      </c>
-      <c r="E28" s="8">
-        <v>143.00219999999999</v>
+      <c r="B30" s="8">
+        <v>985.7568</v>
+      </c>
+      <c r="C30" s="8">
+        <v>6683.2475999999997</v>
+      </c>
+      <c r="D30" s="8">
+        <v>39.7791</v>
+      </c>
+      <c r="E30" s="8">
+        <v>122.9037</v>
       </c>
     </row>
   </sheetData>
@@ -1480,29 +1551,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{701443B9-BE08-4453-A81C-8F690E1F6098}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="A26:E26"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1525,7 +1596,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1548,7 +1619,7 @@
         <v>66321</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1571,7 +1642,7 @@
         <v>6129</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>10</v>
       </c>
@@ -1588,7 +1659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1605,14 +1676,14 @@
         <v>188.1241</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1621,7 +1692,7 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
@@ -1639,7 +1710,7 @@
       </c>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -1656,7 +1727,7 @@
         <v>307.42380000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -1673,7 +1744,7 @@
         <v>96.766499999999994</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -1690,7 +1761,7 @@
         <v>89.116100000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1707,7 +1778,7 @@
         <v>277.24020000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>13</v>
       </c>
@@ -1724,14 +1795,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -1740,7 +1811,7 @@
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>0</v>
       </c>
@@ -1763,203 +1834,237 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>1</v>
       </c>
       <c r="B18" s="8">
-        <v>6386.0460999999996</v>
+        <v>3325.4703</v>
       </c>
       <c r="C18" s="8">
-        <v>7009.5599000000002</v>
+        <v>2065.9158000000002</v>
       </c>
       <c r="D18" s="8">
-        <v>697.88570000000004</v>
+        <v>174.0326</v>
       </c>
       <c r="E18" s="8">
-        <v>180.3689</v>
+        <v>117.1032</v>
       </c>
       <c r="G18" t="s">
         <v>18</v>
       </c>
       <c r="H18" s="8">
-        <v>7073</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="8">
-        <v>5696.6977999999999</v>
-      </c>
-      <c r="C19" s="8">
-        <v>6832.9148999999998</v>
-      </c>
-      <c r="D19" s="8">
-        <v>8.5373999999999999</v>
-      </c>
-      <c r="E19" s="8">
-        <v>3.7239</v>
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>3313.2152999999998</v>
+      </c>
+      <c r="C19">
+        <v>2029.0075999999999</v>
+      </c>
+      <c r="D19">
+        <v>161.77760000000001</v>
+      </c>
+      <c r="E19">
+        <v>80.194999999999894</v>
       </c>
       <c r="G19" t="s">
         <v>19</v>
       </c>
-      <c r="H19" s="8">
-        <v>6876</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="12" t="s">
+      <c r="H19" s="9">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="8">
+        <v>3152.7809000000002</v>
+      </c>
+      <c r="C20" s="8">
+        <v>1948.8126</v>
+      </c>
+      <c r="D20" s="8">
+        <v>1.34320000000025</v>
+      </c>
+      <c r="E20" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="13">
-        <v>5688.1603999999998</v>
-      </c>
-      <c r="C20" s="13">
-        <v>6829.1909999999998</v>
-      </c>
-      <c r="D20" s="13">
-        <v>0</v>
-      </c>
-      <c r="E20" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+      <c r="B21" s="13">
+        <v>3151.4376999999999</v>
+      </c>
+      <c r="C21" s="13">
+        <v>1953.104</v>
+      </c>
+      <c r="D21" s="13">
+        <v>0</v>
+      </c>
+      <c r="E21" s="13">
+        <v>4.2914000000000696</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="8">
-        <v>6227.3860999999997</v>
-      </c>
-      <c r="C21" s="8">
-        <v>6977.2822999999999</v>
-      </c>
-      <c r="D21" s="8">
-        <v>539.22569999999996</v>
-      </c>
-      <c r="E21" s="8">
-        <v>148.09129999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="3"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" s="9"/>
+      <c r="B22" s="8">
+        <v>3306.5147999999999</v>
+      </c>
+      <c r="C22" s="8">
+        <v>2029.2448999999999</v>
+      </c>
+      <c r="D22" s="8">
+        <v>155.0771</v>
+      </c>
+      <c r="E22" s="8">
+        <v>80.432299999999898</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="10" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D25" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E25" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G25" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="H25" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="3">
-        <v>1</v>
-      </c>
-      <c r="B25" s="8">
-        <v>1314.7762</v>
-      </c>
-      <c r="C25" s="8">
-        <v>2636.5578999999998</v>
-      </c>
-      <c r="D25" s="8">
-        <v>171.17330000000001</v>
-      </c>
-      <c r="E25" s="8">
-        <v>40.764200000000002</v>
-      </c>
-      <c r="G25" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>1</v>
+      </c>
+      <c r="B26" s="8">
+        <v>1076.9756</v>
+      </c>
+      <c r="C26" s="8">
+        <v>1643.2242000000001</v>
+      </c>
+      <c r="D26" s="8">
+        <v>152.8399</v>
+      </c>
+      <c r="E26" s="8">
+        <v>109.87390000000001</v>
+      </c>
+      <c r="G26" t="s">
         <v>18</v>
       </c>
-      <c r="H25" s="8">
-        <v>2363</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="12" t="s">
+      <c r="H26" s="9">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27">
+        <v>1083.0374999999999</v>
+      </c>
+      <c r="C27">
+        <v>1652.2330999999999</v>
+      </c>
+      <c r="D27">
+        <v>158.90180000000001</v>
+      </c>
+      <c r="E27">
+        <v>118.8828</v>
+      </c>
+      <c r="G27" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" s="8">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="13">
-        <v>1143.6029000000001</v>
-      </c>
-      <c r="C26" s="13">
-        <v>2595.7937000000002</v>
-      </c>
-      <c r="D26" s="13">
-        <v>0</v>
-      </c>
-      <c r="E26" s="13">
-        <v>0</v>
-      </c>
-      <c r="G26" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="8">
-        <v>2352</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
+      <c r="B28" s="13">
+        <v>924.13570000000004</v>
+      </c>
+      <c r="C28" s="13">
+        <v>1533.3503000000001</v>
+      </c>
+      <c r="D28" s="13">
+        <v>0</v>
+      </c>
+      <c r="E28" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="8">
-        <v>1148.5463</v>
-      </c>
-      <c r="C27" s="8">
-        <v>2603.7049000000002</v>
-      </c>
-      <c r="D27" s="8">
-        <v>4.9433999999999996</v>
-      </c>
-      <c r="E27" s="8">
-        <v>7.9112</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
+      <c r="B29" s="8">
+        <v>929.95709999999997</v>
+      </c>
+      <c r="C29" s="8">
+        <v>1541.1669999999999</v>
+      </c>
+      <c r="D29" s="8">
+        <v>5.8213999999999304</v>
+      </c>
+      <c r="E29" s="8">
+        <v>7.8166999999998596</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="8">
-        <v>1324.3126</v>
-      </c>
-      <c r="C28" s="8">
-        <v>2652.788</v>
-      </c>
-      <c r="D28" s="8">
-        <v>180.7097</v>
-      </c>
-      <c r="E28" s="8">
-        <v>56.994300000000003</v>
+      <c r="B30" s="8">
+        <v>1087.7777000000001</v>
+      </c>
+      <c r="C30" s="8">
+        <v>1661.6324</v>
+      </c>
+      <c r="D30" s="8">
+        <v>163.642</v>
+      </c>
+      <c r="E30" s="8">
+        <v>128.28210000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1969,29 +2074,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{554815FD-A97D-4D1A-B16F-DD10A7B7B7DE}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.36328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -2014,7 +2119,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -2037,7 +2142,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -2060,7 +2165,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>10</v>
       </c>
@@ -2077,7 +2182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -2094,16 +2199,16 @@
         <v>74.208200000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="9"/>
     </row>
-    <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>0</v>
       </c>
@@ -2121,7 +2226,7 @@
       </c>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2138,7 +2243,7 @@
         <v>93.695900000000194</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2155,7 +2260,7 @@
         <v>3.8375000000000901</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2172,7 +2277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -2189,7 +2294,7 @@
         <v>74.208200000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>13</v>
       </c>
@@ -2206,16 +2311,16 @@
         <v>22.251799999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="9"/>
     </row>
-    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>0</v>
       </c>
@@ -2238,192 +2343,230 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>1</v>
       </c>
       <c r="B18" s="8">
-        <v>3201.3962000000001</v>
+        <v>1413.3135</v>
       </c>
       <c r="C18" s="8">
-        <v>2680.9920000000002</v>
+        <v>606.75009999999997</v>
       </c>
       <c r="D18" s="8">
-        <v>122.0162</v>
+        <v>106.6324</v>
       </c>
       <c r="E18" s="8">
-        <v>105.5519</v>
+        <v>0</v>
       </c>
       <c r="G18" t="s">
         <v>18</v>
       </c>
       <c r="H18" s="8">
-        <v>906</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="13">
-        <v>3079.38</v>
-      </c>
-      <c r="C19" s="13">
-        <v>2578.2813999999998</v>
-      </c>
-      <c r="D19" s="13">
-        <v>0</v>
-      </c>
-      <c r="E19" s="13">
-        <v>2.8412999999999999</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="8">
+        <v>1391.306</v>
+      </c>
+      <c r="C19" s="8">
+        <v>621.82830000000001</v>
+      </c>
+      <c r="D19" s="8">
+        <v>84.624899999999997</v>
+      </c>
+      <c r="E19" s="8">
+        <v>15.078200000000001</v>
       </c>
       <c r="G19" t="s">
         <v>19</v>
       </c>
-      <c r="H19" s="8">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H19" s="9">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="13">
+        <v>1310.2048</v>
+      </c>
+      <c r="C20" s="13">
+        <v>615.38930000000005</v>
+      </c>
+      <c r="D20" s="13">
+        <v>3.5236999999999599</v>
+      </c>
+      <c r="E20" s="13">
+        <v>8.6392000000000699</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="13">
-        <v>3084.8337000000001</v>
-      </c>
-      <c r="C20" s="13">
-        <v>2575.4400999999998</v>
-      </c>
-      <c r="D20" s="13">
-        <v>5.4537000000000004</v>
-      </c>
-      <c r="E20" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+      <c r="B21" s="13">
+        <v>1306.6811</v>
+      </c>
+      <c r="C21" s="13">
+        <v>617.18949999999995</v>
+      </c>
+      <c r="D21" s="13">
+        <v>0</v>
+      </c>
+      <c r="E21" s="13">
+        <v>10.439399999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="8">
-        <v>3160.0922</v>
-      </c>
-      <c r="C21" s="8">
-        <v>2645.29</v>
-      </c>
-      <c r="D21" s="8">
-        <v>80.712199999999996</v>
-      </c>
-      <c r="E21" s="8">
-        <v>69.849900000000005</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="3"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
+      <c r="B22" s="8">
+        <v>1390.5564999999999</v>
+      </c>
+      <c r="C22" s="8">
+        <v>624.92610000000002</v>
+      </c>
+      <c r="D22" s="8">
+        <v>83.8753999999999</v>
+      </c>
+      <c r="E22" s="8">
+        <v>18.175999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="9"/>
-    </row>
-    <row r="24" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="11" t="s">
+      <c r="B24" s="9"/>
+    </row>
+    <row r="25" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D25" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E25" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G25" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="H25" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="3">
-        <v>1</v>
-      </c>
-      <c r="B25" s="8">
-        <v>1422.578</v>
-      </c>
-      <c r="C25" s="8">
-        <v>1886.934</v>
-      </c>
-      <c r="D25" s="8">
-        <v>55.244399999999999</v>
-      </c>
-      <c r="E25" s="8">
-        <v>241.13030000000001</v>
-      </c>
-      <c r="G25" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>1</v>
+      </c>
+      <c r="B26" s="8">
+        <v>1094.1410000000001</v>
+      </c>
+      <c r="C26" s="8">
+        <v>1121.7267999999999</v>
+      </c>
+      <c r="D26" s="8">
+        <v>95.442600000000098</v>
+      </c>
+      <c r="E26" s="8">
+        <v>130.2089</v>
+      </c>
+      <c r="G26" t="s">
         <v>18</v>
       </c>
-      <c r="H25" s="8"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="12" t="s">
+      <c r="H26" s="8">
+        <v>-52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="8">
+        <v>1091.5263</v>
+      </c>
+      <c r="C27" s="8">
+        <v>1101.2979</v>
+      </c>
+      <c r="D27" s="8">
+        <v>92.8279</v>
+      </c>
+      <c r="E27" s="8">
+        <v>109.78</v>
+      </c>
+      <c r="G27" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" s="9">
+        <v>-99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="13">
-        <v>1367.3335999999999</v>
-      </c>
-      <c r="C26" s="13">
-        <v>1645.8036999999999</v>
-      </c>
-      <c r="D26" s="13">
-        <v>0</v>
-      </c>
-      <c r="E26" s="13">
-        <v>0</v>
-      </c>
-      <c r="G26" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="8"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
+      <c r="B28" s="13">
+        <v>998.69839999999999</v>
+      </c>
+      <c r="C28" s="13">
+        <v>991.51790000000005</v>
+      </c>
+      <c r="D28" s="13">
+        <v>0</v>
+      </c>
+      <c r="E28" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="8">
-        <v>1373.8653999999999</v>
-      </c>
-      <c r="C27" s="8">
-        <v>1651.5381</v>
-      </c>
-      <c r="D27" s="8">
-        <v>6.5317999999999996</v>
-      </c>
-      <c r="E27" s="8">
-        <v>5.7343999999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
+      <c r="B29" s="8">
+        <v>1001.1322</v>
+      </c>
+      <c r="C29" s="8">
+        <v>995.61760000000004</v>
+      </c>
+      <c r="D29" s="8">
+        <v>2.4338000000000202</v>
+      </c>
+      <c r="E29" s="8">
+        <v>4.0996999999999799</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="8">
-        <v>1432.6815999999999</v>
-      </c>
-      <c r="C28" s="8">
-        <v>1850.4525000000001</v>
-      </c>
-      <c r="D28" s="8">
-        <v>65.347999999999999</v>
-      </c>
-      <c r="E28" s="8">
-        <v>204.64879999999999</v>
+      <c r="B30" s="8">
+        <v>1094.7583999999999</v>
+      </c>
+      <c r="C30" s="8">
+        <v>1106.7331999999999</v>
+      </c>
+      <c r="D30" s="8">
+        <v>96.059999999999903</v>
+      </c>
+      <c r="E30" s="8">
+        <v>115.2153</v>
       </c>
     </row>
   </sheetData>
@@ -2433,29 +2576,29 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37CA56D-4361-434A-9E6E-71922355AB0B}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.26953125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.90625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -2478,7 +2621,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2501,7 +2644,7 @@
         <v>9797</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2524,7 +2667,7 @@
         <v>9306</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>10</v>
       </c>
@@ -2541,7 +2684,7 @@
         <v>0.8619</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2558,16 +2701,16 @@
         <v>302.43689999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="9"/>
     </row>
-    <row r="9" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>0</v>
       </c>
@@ -2586,7 +2729,7 @@
       <c r="G9" s="10"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -2603,7 +2746,7 @@
         <v>470.94459999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -2620,7 +2763,7 @@
         <v>69.024199999999993</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -2637,7 +2780,7 @@
         <v>69.886099999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -2654,7 +2797,7 @@
         <v>371.46109999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>13</v>
       </c>
@@ -2671,16 +2814,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="9"/>
     </row>
-    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>0</v>
       </c>
@@ -2703,196 +2846,230 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18" s="8">
-        <v>10075.69</v>
+        <v>7031.9184999999998</v>
       </c>
       <c r="C18" s="8">
-        <v>11938.187900000001</v>
+        <v>5758.2276000000002</v>
       </c>
       <c r="D18" s="8">
-        <v>441.81509999999997</v>
+        <v>268.78059999999999</v>
       </c>
       <c r="E18" s="8">
-        <v>357.38870000000099</v>
+        <v>152.99600000000001</v>
       </c>
       <c r="G18" t="s">
         <v>18</v>
       </c>
       <c r="H18" s="8">
-        <v>10704</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+        <v>5008</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B19" s="8">
-        <v>9664.9472000000005</v>
+        <v>6938.0177999999996</v>
       </c>
       <c r="C19" s="8">
-        <v>11580.799199999999</v>
+        <v>5709.3629000000001</v>
       </c>
       <c r="D19" s="8">
-        <v>31.0722999999998</v>
+        <v>174.87989999999999</v>
       </c>
       <c r="E19" s="8">
-        <v>0</v>
+        <v>104.1313</v>
       </c>
       <c r="G19" t="s">
         <v>19</v>
       </c>
-      <c r="H19" s="8">
-        <v>10210</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="14" t="s">
+      <c r="H19" s="9">
+        <v>4789</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="8">
+        <v>6789.8014000000003</v>
+      </c>
+      <c r="C20" s="8">
+        <v>5605.2316000000001</v>
+      </c>
+      <c r="D20" s="8">
+        <v>26.663500000000599</v>
+      </c>
+      <c r="E20" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="13">
-        <v>9633.8749000000007</v>
-      </c>
-      <c r="C20" s="13">
-        <v>11581.541300000001</v>
-      </c>
-      <c r="D20" s="13">
-        <v>0</v>
-      </c>
-      <c r="E20" s="13">
-        <v>0.74210000000130105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="B21" s="13">
+        <v>6763.1378999999997</v>
+      </c>
+      <c r="C21" s="13">
+        <v>5608.4396999999999</v>
+      </c>
+      <c r="D21" s="13">
+        <v>0</v>
+      </c>
+      <c r="E21" s="13">
+        <v>3.2080999999998299</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="8">
-        <v>9833.5134999999991</v>
-      </c>
-      <c r="C21" s="8">
-        <v>11822.6998</v>
-      </c>
-      <c r="D21" s="8">
-        <v>199.63859999999801</v>
-      </c>
-      <c r="E21" s="8">
-        <v>241.90060000000099</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="3"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
+      <c r="B22" s="8">
+        <v>6913.0578999999998</v>
+      </c>
+      <c r="C22" s="8">
+        <v>5712.5971</v>
+      </c>
+      <c r="D22" s="8">
+        <v>149.91999999999999</v>
+      </c>
+      <c r="E22" s="8">
+        <v>107.3655</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="9"/>
-    </row>
-    <row r="24" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="10" t="s">
+      <c r="B24" s="9"/>
+    </row>
+    <row r="25" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D25" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E25" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G25" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="H25" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="3">
-        <v>1</v>
-      </c>
-      <c r="B25" s="8">
-        <v>1439.2109</v>
-      </c>
-      <c r="C25" s="8">
-        <v>3924.2869999999998</v>
-      </c>
-      <c r="D25" s="8">
-        <v>89.943299999999994</v>
-      </c>
-      <c r="E25" s="8">
-        <v>308.58870000000002</v>
-      </c>
-      <c r="G25" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>1</v>
+      </c>
+      <c r="B26" s="8">
+        <v>1350.2887000000001</v>
+      </c>
+      <c r="C26" s="8">
+        <v>3481.3643999999999</v>
+      </c>
+      <c r="D26" s="8">
+        <v>115.38890000000001</v>
+      </c>
+      <c r="E26" s="8">
+        <v>255.97030000000001</v>
+      </c>
+      <c r="G26" t="s">
         <v>18</v>
       </c>
-      <c r="H25" s="8">
-        <v>3604</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
+      <c r="H26" s="9">
+        <v>3217</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="8">
+        <v>1308.9353000000001</v>
+      </c>
+      <c r="C27" s="8">
+        <v>3424.0047</v>
+      </c>
+      <c r="D27" s="8">
+        <v>74.035500000000198</v>
+      </c>
+      <c r="E27" s="8">
+        <v>198.61060000000001</v>
+      </c>
+      <c r="G27" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" s="8">
+        <v>3268</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="8">
-        <v>1349.2675999999999</v>
-      </c>
-      <c r="C26" s="8">
-        <v>3627.7406999999998</v>
-      </c>
-      <c r="D26" s="8">
-        <v>0</v>
-      </c>
-      <c r="E26" s="8">
-        <v>12.042400000000001</v>
-      </c>
-      <c r="G26" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="8">
-        <v>3617</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="12" t="s">
+      <c r="B28" s="8">
+        <v>1234.8997999999999</v>
+      </c>
+      <c r="C28" s="8">
+        <v>3234.8670000000002</v>
+      </c>
+      <c r="D28" s="8">
+        <v>0</v>
+      </c>
+      <c r="E28" s="8">
+        <v>9.4729000000002106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="13">
-        <v>1352.1359</v>
-      </c>
-      <c r="C27" s="13">
-        <v>3615.6983</v>
-      </c>
-      <c r="D27" s="13">
-        <v>2.8683000000000001</v>
-      </c>
-      <c r="E27" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
+      <c r="B29" s="13">
+        <v>1236.7474999999999</v>
+      </c>
+      <c r="C29" s="13">
+        <v>3225.3941</v>
+      </c>
+      <c r="D29" s="13">
+        <v>1.8477000000000301</v>
+      </c>
+      <c r="E29" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="8">
-        <v>1409.2742000000001</v>
-      </c>
-      <c r="C28" s="8">
-        <v>3850.0315999999998</v>
-      </c>
-      <c r="D28" s="8">
-        <v>60.006599999999999</v>
-      </c>
-      <c r="E28" s="8">
-        <v>234.33330000000001</v>
+      <c r="B30" s="8">
+        <v>1312.1496</v>
+      </c>
+      <c r="C30" s="8">
+        <v>3423.7701000000002</v>
+      </c>
+      <c r="D30" s="8">
+        <v>77.249800000000107</v>
+      </c>
+      <c r="E30" s="8">
+        <v>198.376</v>
       </c>
     </row>
   </sheetData>
@@ -2902,29 +3079,29 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04802266-9949-4C25-9707-E66188161F44}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J12:J13"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.26953125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.90625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2948,7 +3125,7 @@
       </c>
       <c r="I2" s="11"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -2971,7 +3148,7 @@
         <v>7147</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -2994,7 +3171,7 @@
         <v>6580</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>10</v>
       </c>
@@ -3011,7 +3188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -3028,16 +3205,16 @@
         <v>205.94649999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="9"/>
     </row>
-    <row r="9" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
@@ -3055,7 +3232,7 @@
       </c>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -3072,7 +3249,7 @@
         <v>485.53629999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -3089,7 +3266,7 @@
         <v>83.571600000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -3106,7 +3283,7 @@
         <v>13.009499999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -3123,7 +3300,7 @@
         <v>218.95599999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>13</v>
       </c>
@@ -3140,16 +3317,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="9"/>
     </row>
-    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>0</v>
       </c>
@@ -3172,196 +3349,230 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>1</v>
       </c>
       <c r="B18" s="8">
-        <v>9610.7330000000002</v>
+        <v>6983.7155000000002</v>
       </c>
       <c r="C18" s="8">
-        <v>10838.5807</v>
+        <v>5513.1688000000004</v>
       </c>
       <c r="D18" s="8">
-        <v>756.53689999999995</v>
+        <v>772.91589999999997</v>
       </c>
       <c r="E18" s="8">
-        <v>537.28719999999998</v>
+        <v>279.69050000000101</v>
       </c>
       <c r="G18" t="s">
         <v>18</v>
       </c>
       <c r="H18" s="8">
-        <v>7942</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
-        <v>5</v>
+        <v>3732</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>21</v>
       </c>
       <c r="B19" s="8">
-        <v>8924.3956999999991</v>
+        <v>6639.7658000000001</v>
       </c>
       <c r="C19" s="8">
-        <v>10378.42</v>
+        <v>5402.2851000000001</v>
       </c>
       <c r="D19" s="8">
-        <v>70.199600000000004</v>
+        <v>428.96620000000001</v>
       </c>
       <c r="E19" s="8">
-        <v>77.126499999999993</v>
+        <v>168.80680000000001</v>
       </c>
       <c r="G19" t="s">
         <v>19</v>
       </c>
-      <c r="H19" s="8">
-        <v>7345</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="12" t="s">
+      <c r="H19" s="9">
+        <v>3437</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="8">
+        <v>6252.3375999999998</v>
+      </c>
+      <c r="C20" s="8">
+        <v>5280.7209999999995</v>
+      </c>
+      <c r="D20" s="8">
+        <v>41.537999999999599</v>
+      </c>
+      <c r="E20" s="8">
+        <v>47.2426999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="13">
-        <v>8854.1960999999992</v>
-      </c>
-      <c r="C20" s="13">
-        <v>10301.2935</v>
-      </c>
-      <c r="D20" s="13">
-        <v>0</v>
-      </c>
-      <c r="E20" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+      <c r="B21" s="13">
+        <v>6210.7996000000003</v>
+      </c>
+      <c r="C21" s="13">
+        <v>5233.4782999999998</v>
+      </c>
+      <c r="D21" s="13">
+        <v>0</v>
+      </c>
+      <c r="E21" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="8">
-        <v>9201.3667000000005</v>
-      </c>
-      <c r="C21" s="8">
-        <v>10561.380999999999</v>
-      </c>
-      <c r="D21" s="8">
-        <v>347.17059999999998</v>
-      </c>
-      <c r="E21" s="8">
-        <v>260.08749999999998</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="3"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
+      <c r="B22" s="8">
+        <v>6593.0097999999998</v>
+      </c>
+      <c r="C22" s="8">
+        <v>5354.5225</v>
+      </c>
+      <c r="D22" s="8">
+        <v>382.21019999999999</v>
+      </c>
+      <c r="E22" s="8">
+        <v>121.0442</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="9"/>
-    </row>
-    <row r="24" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="10" t="s">
+      <c r="B24" s="9"/>
+    </row>
+    <row r="25" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D25" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E25" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G25" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="H25" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="3">
-        <v>1</v>
-      </c>
-      <c r="B25" s="8">
-        <v>1383.0856000000001</v>
-      </c>
-      <c r="C25" s="8">
-        <v>4803.6590999999999</v>
-      </c>
-      <c r="D25" s="8">
-        <v>200.78020000000001</v>
-      </c>
-      <c r="E25" s="8">
-        <v>846.07889999999998</v>
-      </c>
-      <c r="G25" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>1</v>
+      </c>
+      <c r="B26" s="8">
+        <v>1320.5497</v>
+      </c>
+      <c r="C26" s="8">
+        <v>4101.8912</v>
+      </c>
+      <c r="D26" s="8">
+        <v>258.72109999999998</v>
+      </c>
+      <c r="E26" s="8">
+        <v>666.45680000000004</v>
+      </c>
+      <c r="G26" t="s">
         <v>18</v>
       </c>
-      <c r="H25" s="8">
-        <v>2883</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
+      <c r="H26" s="8">
+        <v>2831</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="8">
+        <v>1269.337</v>
+      </c>
+      <c r="C27" s="8">
+        <v>3928.4843999999998</v>
+      </c>
+      <c r="D27" s="8">
+        <v>207.50839999999999</v>
+      </c>
+      <c r="E27" s="8">
+        <v>493.05</v>
+      </c>
+      <c r="G27" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" s="9">
+        <v>2826</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="8">
-        <v>1195.0506</v>
-      </c>
-      <c r="C26" s="8">
-        <v>3984.4020999999998</v>
-      </c>
-      <c r="D26" s="8">
-        <v>12.745200000000001</v>
-      </c>
-      <c r="E26" s="8">
-        <v>26.821899999999999</v>
-      </c>
-      <c r="G26" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="8">
-        <v>2848</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="12" t="s">
+      <c r="B28" s="8">
+        <v>1081.8733999999999</v>
+      </c>
+      <c r="C28" s="8">
+        <v>3464.4400999999998</v>
+      </c>
+      <c r="D28" s="8">
+        <v>20.044799999999899</v>
+      </c>
+      <c r="E28" s="8">
+        <v>29.005699999999699</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="13">
-        <v>1182.3054</v>
-      </c>
-      <c r="C27" s="13">
-        <v>3957.5801999999999</v>
-      </c>
-      <c r="D27" s="13">
-        <v>0</v>
-      </c>
-      <c r="E27" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
+      <c r="B29" s="13">
+        <v>1061.8286000000001</v>
+      </c>
+      <c r="C29" s="13">
+        <v>3435.4344000000001</v>
+      </c>
+      <c r="D29" s="13">
+        <v>0</v>
+      </c>
+      <c r="E29" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="8">
-        <v>1326.7722000000001</v>
-      </c>
-      <c r="C28" s="8">
-        <v>4587.0888999999997</v>
-      </c>
-      <c r="D28" s="8">
-        <v>144.46680000000001</v>
-      </c>
-      <c r="E28" s="8">
-        <v>629.50869999999998</v>
+      <c r="B30" s="8">
+        <v>1256.6600000000001</v>
+      </c>
+      <c r="C30" s="8">
+        <v>3907.7280000000001</v>
+      </c>
+      <c r="D30" s="8">
+        <v>194.8314</v>
+      </c>
+      <c r="E30" s="8">
+        <v>472.29360000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>